<commit_message>
MJ818 SuperNova Mini2: - added position key into PCB and spacers; updated gerber, dwg and stl
mj513 - grip:
- corrected bushing dimensions

in mj8x8-foo:
- minor corrections

general board-wide effort:
- replaced pinhead with 0.9mm TH
- added 2nd CAN H & L solder contact
- unified sch nets and drawings

in mj8x8 foo:
- developed rev.1b mj-foo device with voltage detector and CAN TVS protection

in mj808 design:
- updated front led shunt resistor to 0.18 Ohm

in mj8x8:
- added HR30-6R-6P - PushPull Receptacle.lbr receptable
</commit_message>
<xml_diff>
--- a/eagle design/mj808/BOM MJ808 clone - rev.5 - TCAN334 - SN E3 - prod.xlsx
+++ b/eagle design/mj808/BOM MJ808 clone - rev.5 - TCAN334 - SN E3 - prod.xlsx
@@ -201,9 +201,6 @@
     <t>LED702</t>
   </si>
   <si>
-    <t>WSLT2010R2200FEB18 / 0.22Ohm 1W</t>
-  </si>
-  <si>
     <t>R-EU_R2010</t>
   </si>
   <si>
@@ -249,10 +246,6 @@
     <t>https://hr.mouser.com/ProductDetail/604-WP7113VRVC1C</t>
   </si>
   <si>
-    <t>71-RCWE1210R150FKEA
-71-RCWE1210R180FKEA</t>
-  </si>
-  <si>
     <t>595-TCAN334GDCNT</t>
   </si>
   <si>
@@ -329,6 +322,12 @@
   </si>
   <si>
     <t>https://hr.mouser.com/ProductDetail/Cree-LED/XMLBWT-00-0000-0000U20E2?qs=5YqktSXERioTBWgw3sCLZA%3D%3D</t>
+  </si>
+  <si>
+    <t>71-RCWE1210R180FKEA</t>
+  </si>
+  <si>
+    <t>RCWE1210R180FKEA  / 0.18Ohm 1W</t>
   </si>
 </sst>
 </file>
@@ -694,8 +693,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -730,10 +729,10 @@
         <v>5</v>
       </c>
       <c r="G1" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="H1" s="4" t="s">
         <v>66</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -756,10 +755,10 @@
         <v>10</v>
       </c>
       <c r="G2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -767,7 +766,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C3" t="s">
         <v>11</v>
@@ -782,10 +781,10 @@
         <v>14</v>
       </c>
       <c r="G3" t="s">
+        <v>68</v>
+      </c>
+      <c r="H3" s="6" t="s">
         <v>69</v>
-      </c>
-      <c r="H3" s="6" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -802,16 +801,16 @@
         <v>8</v>
       </c>
       <c r="E4" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="F4" t="s">
         <v>10</v>
       </c>
       <c r="G4" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="H4" s="6" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -834,10 +833,10 @@
         <v>10</v>
       </c>
       <c r="G5" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="H5" s="6" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -845,7 +844,7 @@
         <v>2</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C6" t="s">
         <v>18</v>
@@ -860,10 +859,10 @@
         <v>14</v>
       </c>
       <c r="G6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H6" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -883,10 +882,10 @@
         <v>24</v>
       </c>
       <c r="G7" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="H7" s="6" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -906,10 +905,10 @@
         <v>28</v>
       </c>
       <c r="G8" t="s">
+        <v>71</v>
+      </c>
+      <c r="H8" s="6" t="s">
         <v>72</v>
-      </c>
-      <c r="H8" s="6" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -929,10 +928,10 @@
         <v>31</v>
       </c>
       <c r="G9" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="H9" s="6" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -952,10 +951,10 @@
         <v>35</v>
       </c>
       <c r="G10" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="H10" s="6" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -978,10 +977,10 @@
         <v>40</v>
       </c>
       <c r="G11" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="H11" s="6" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -1001,10 +1000,10 @@
         <v>44</v>
       </c>
       <c r="G12" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="H12" s="6" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -1024,10 +1023,10 @@
         <v>48</v>
       </c>
       <c r="G13" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="H13" s="6" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -1047,10 +1046,10 @@
         <v>52</v>
       </c>
       <c r="G14" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="H14" s="6" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -1073,10 +1072,10 @@
         <v>57</v>
       </c>
       <c r="G15" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="H15" s="6" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -1096,33 +1095,33 @@
         <v>59</v>
       </c>
       <c r="G16" t="s">
+        <v>73</v>
+      </c>
+      <c r="H16" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="H16" s="6" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>1</v>
       </c>
       <c r="B17" t="s">
+        <v>102</v>
+      </c>
+      <c r="C17" t="s">
         <v>60</v>
       </c>
-      <c r="C17" t="s">
+      <c r="D17" t="s">
         <v>61</v>
       </c>
-      <c r="D17" t="s">
+      <c r="E17" t="s">
         <v>62</v>
-      </c>
-      <c r="E17" t="s">
-        <v>63</v>
       </c>
       <c r="F17" t="s">
         <v>14</v>
       </c>
       <c r="G17" s="7" t="s">
-        <v>76</v>
+        <v>101</v>
       </c>
       <c r="H17" s="6"/>
     </row>
@@ -1131,13 +1130,13 @@
         <v>1</v>
       </c>
       <c r="C18" t="s">
+        <v>98</v>
+      </c>
+      <c r="G18" t="s">
+        <v>99</v>
+      </c>
+      <c r="H18" s="6" t="s">
         <v>100</v>
-      </c>
-      <c r="G18" t="s">
-        <v>101</v>
-      </c>
-      <c r="H18" s="6" t="s">
-        <v>102</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
general board-wide effort: - replaced pinhead with 0.9mm TH - added 2nd CAN H & L solder contact - unified sch nets and drawings
in mj8x8 foo:
- developed rev.1b mj-foo device with voltage detector and CAN TVS protection

in mj808 design:
- updated front led shunt resistor to 0.18 Ohm
</commit_message>
<xml_diff>
--- a/eagle design/mj808/BOM MJ808 clone - rev.5 - TCAN334 - SN E3 - prod.xlsx
+++ b/eagle design/mj808/BOM MJ808 clone - rev.5 - TCAN334 - SN E3 - prod.xlsx
@@ -201,9 +201,6 @@
     <t>LED702</t>
   </si>
   <si>
-    <t>WSLT2010R2200FEB18 / 0.22Ohm 1W</t>
-  </si>
-  <si>
     <t>R-EU_R2010</t>
   </si>
   <si>
@@ -249,10 +246,6 @@
     <t>https://hr.mouser.com/ProductDetail/604-WP7113VRVC1C</t>
   </si>
   <si>
-    <t>71-RCWE1210R150FKEA
-71-RCWE1210R180FKEA</t>
-  </si>
-  <si>
     <t>595-TCAN334GDCNT</t>
   </si>
   <si>
@@ -329,6 +322,12 @@
   </si>
   <si>
     <t>https://hr.mouser.com/ProductDetail/Cree-LED/XMLBWT-00-0000-0000U20E2?qs=5YqktSXERioTBWgw3sCLZA%3D%3D</t>
+  </si>
+  <si>
+    <t>71-RCWE1210R180FKEA</t>
+  </si>
+  <si>
+    <t>RCWE1210R180FKEA  / 0.18Ohm 1W</t>
   </si>
 </sst>
 </file>
@@ -694,8 +693,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -730,10 +729,10 @@
         <v>5</v>
       </c>
       <c r="G1" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="H1" s="4" t="s">
         <v>66</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -756,10 +755,10 @@
         <v>10</v>
       </c>
       <c r="G2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -767,7 +766,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C3" t="s">
         <v>11</v>
@@ -782,10 +781,10 @@
         <v>14</v>
       </c>
       <c r="G3" t="s">
+        <v>68</v>
+      </c>
+      <c r="H3" s="6" t="s">
         <v>69</v>
-      </c>
-      <c r="H3" s="6" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -802,16 +801,16 @@
         <v>8</v>
       </c>
       <c r="E4" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="F4" t="s">
         <v>10</v>
       </c>
       <c r="G4" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="H4" s="6" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -834,10 +833,10 @@
         <v>10</v>
       </c>
       <c r="G5" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="H5" s="6" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -845,7 +844,7 @@
         <v>2</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C6" t="s">
         <v>18</v>
@@ -860,10 +859,10 @@
         <v>14</v>
       </c>
       <c r="G6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H6" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -883,10 +882,10 @@
         <v>24</v>
       </c>
       <c r="G7" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="H7" s="6" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -906,10 +905,10 @@
         <v>28</v>
       </c>
       <c r="G8" t="s">
+        <v>71</v>
+      </c>
+      <c r="H8" s="6" t="s">
         <v>72</v>
-      </c>
-      <c r="H8" s="6" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -929,10 +928,10 @@
         <v>31</v>
       </c>
       <c r="G9" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="H9" s="6" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -952,10 +951,10 @@
         <v>35</v>
       </c>
       <c r="G10" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="H10" s="6" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -978,10 +977,10 @@
         <v>40</v>
       </c>
       <c r="G11" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="H11" s="6" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -1001,10 +1000,10 @@
         <v>44</v>
       </c>
       <c r="G12" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="H12" s="6" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -1024,10 +1023,10 @@
         <v>48</v>
       </c>
       <c r="G13" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="H13" s="6" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -1047,10 +1046,10 @@
         <v>52</v>
       </c>
       <c r="G14" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="H14" s="6" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -1073,10 +1072,10 @@
         <v>57</v>
       </c>
       <c r="G15" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="H15" s="6" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -1096,33 +1095,33 @@
         <v>59</v>
       </c>
       <c r="G16" t="s">
+        <v>73</v>
+      </c>
+      <c r="H16" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="H16" s="6" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>1</v>
       </c>
       <c r="B17" t="s">
+        <v>102</v>
+      </c>
+      <c r="C17" t="s">
         <v>60</v>
       </c>
-      <c r="C17" t="s">
+      <c r="D17" t="s">
         <v>61</v>
       </c>
-      <c r="D17" t="s">
+      <c r="E17" t="s">
         <v>62</v>
-      </c>
-      <c r="E17" t="s">
-        <v>63</v>
       </c>
       <c r="F17" t="s">
         <v>14</v>
       </c>
       <c r="G17" s="7" t="s">
-        <v>76</v>
+        <v>101</v>
       </c>
       <c r="H17" s="6"/>
     </row>
@@ -1131,13 +1130,13 @@
         <v>1</v>
       </c>
       <c r="C18" t="s">
+        <v>98</v>
+      </c>
+      <c r="G18" t="s">
+        <v>99</v>
+      </c>
+      <c r="H18" s="6" t="s">
         <v>100</v>
-      </c>
-      <c r="G18" t="s">
-        <v>101</v>
-      </c>
-      <c r="H18" s="6" t="s">
-        <v>102</v>
       </c>
     </row>
   </sheetData>

</xml_diff>